<commit_message>
Added pie chart to report
</commit_message>
<xml_diff>
--- a/reports/report.xlsx
+++ b/reports/report.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Category Distribution Data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -145,6 +146,95 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Category Distribution</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Category Distribution Data'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Category Distribution Data'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Category Distribution Data'!$B$2:$B$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="1"/>
+          <showCatName val="1"/>
+          <showPercent val="1"/>
+        </dLbls>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>9</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36908,5 +36998,87 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Books</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sports</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>